<commit_message>
Definição de requisitos funcionais e não funcionais
</commit_message>
<xml_diff>
--- a/Documentacao/TI-Backlog.xlsx
+++ b/Documentacao/TI-Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad3eed489a1630f4/Documentos/Faculdade/PESQUISA E INOVAÇÃO/ADS-01/Sprint1/Documentacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="8_{527D46DC-5B78-40FA-8B8B-9F273E6B4D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D745C16-BFD9-43F2-8432-CFE3DB0544FB}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="8_{527D46DC-5B78-40FA-8B8B-9F273E6B4D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A6C1EF5A-ACC9-45FF-920F-663AB4AA63DB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Website</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t>dashboard</t>
+  </si>
+  <si>
+    <t>RNF</t>
+  </si>
+  <si>
+    <t>RF</t>
   </si>
 </sst>
 </file>
@@ -416,26 +422,26 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,6 +457,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>83929</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>58388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97381537-E152-43FB-A15B-84B18542EC1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8282940" y="0"/>
+          <a:ext cx="6096109" cy="2435828"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -719,7 +774,7 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,30 +798,30 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
@@ -793,7 +848,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -804,7 +859,9 @@
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
@@ -820,7 +877,9 @@
       <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
@@ -836,7 +895,9 @@
       <c r="F7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H7" s="1" t="s">
         <v>17</v>
       </c>
@@ -852,7 +913,9 @@
       <c r="F8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
@@ -882,7 +945,9 @@
       <c r="F10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H10" s="1" t="s">
         <v>17</v>
       </c>
@@ -898,7 +963,9 @@
       <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H11" s="1" t="s">
         <v>18</v>
       </c>
@@ -914,7 +981,9 @@
       <c r="F12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>18</v>
       </c>
@@ -930,7 +999,9 @@
       <c r="F13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H13" s="16" t="s">
         <v>18</v>
       </c>
@@ -946,7 +1017,9 @@
       <c r="F14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H14" s="1" t="s">
         <v>18</v>
       </c>
@@ -962,7 +1035,9 @@
       <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H15" s="1" t="s">
         <v>18</v>
       </c>
@@ -992,7 +1067,9 @@
       <c r="F17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1008,7 +1085,9 @@
       <c r="F18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1024,7 +1103,9 @@
       <c r="F19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1054,7 +1135,9 @@
       <c r="F21" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1070,7 +1153,9 @@
       <c r="F22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1086,7 +1171,9 @@
       <c r="F23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H23" s="1" t="s">
         <v>17</v>
       </c>
@@ -1116,7 +1203,9 @@
       <c r="F25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="16"/>
+      <c r="G25" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="H25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1132,7 +1221,9 @@
       <c r="F26" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G26" s="16"/>
+      <c r="G26" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
       </c>
@@ -1241,5 +1332,6 @@
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização no backlog e adicionando a API no repositório
</commit_message>
<xml_diff>
--- a/Documentacao/TI-Backlog.xlsx
+++ b/Documentacao/TI-Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad3eed489a1630f4/Documentos/Faculdade/PESQUISA E INOVAÇÃO/ADS-01/Sprint1/Documentacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\OneDrive\Documentos\Faculdade\PESQUISA E INOVAÇÃO\ADS-01\Sprint1\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="299" documentId="8_{527D46DC-5B78-40FA-8B8B-9F273E6B4D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{844C38DC-856C-4284-8D9E-CE45F25B1387}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2D35AA-842B-4D7D-9660-540D6A8890FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,7 +934,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>9</v>
@@ -952,7 +952,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>9</v>

</xml_diff>